<commit_message>
-Arquivos movidos para pastas corretas
</commit_message>
<xml_diff>
--- a/docs/Cronograma/Cronograma.xlsx
+++ b/docs/Cronograma/Cronograma.xlsx
@@ -1,24 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\_S_Fac\CobrinhaPUC\docs\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3DA9E1-44B4-4AA0-93F5-781E293671D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4963BDA2-3B3D-4B7F-A45A-108EC0090E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma de projeto" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="FIRST_DAY_OF_YEAR">LAMBDA(year, DATE(year,1,1)+CHOOSE(WEEKDAY(DATE(year,1,1),2),0,6,5,4,3,2,1))</definedName>
+    <definedName name="FIRST_DAY_OF_YEAR">_xludf.LAMBDA(year, DATE(year,1,1)+CHOOSE(WEEKDAY(DATE(year,1,1),2),0,6,5,4,3,2,1))</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1124,7 +1137,7 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1475,91 +1488,45 @@
     <xf numFmtId="0" fontId="48" fillId="14" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="12" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="44" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="43" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1573,6 +1540,11 @@
     <xf numFmtId="0" fontId="31" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1589,52 +1561,69 @@
     <xf numFmtId="0" fontId="31" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="12" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="14" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1963,22 +1952,22 @@
   </sheetPr>
   <dimension ref="A1:BM35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="108" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="AZ12" sqref="AZ12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="108" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="BN20" sqref="BN20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.75" customWidth="1"/>
-    <col min="2" max="2" width="9.875" customWidth="1"/>
-    <col min="3" max="3" width="1.375" customWidth="1"/>
-    <col min="4" max="4" width="15.375" customWidth="1"/>
-    <col min="5" max="5" width="10.75" customWidth="1"/>
-    <col min="6" max="7" width="9.375" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="10.25" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="3.765625" customWidth="1"/>
+    <col min="2" max="2" width="9.84375" customWidth="1"/>
+    <col min="3" max="3" width="1.3828125" customWidth="1"/>
+    <col min="4" max="4" width="15.3828125" customWidth="1"/>
+    <col min="5" max="5" width="10.765625" customWidth="1"/>
+    <col min="6" max="7" width="9.3828125" customWidth="1"/>
+    <col min="8" max="8" width="14.4609375" customWidth="1"/>
+    <col min="9" max="9" width="10.23046875" hidden="1" customWidth="1"/>
     <col min="10" max="34" width="3" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="7.125" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="7.15234375" hidden="1" customWidth="1"/>
     <col min="36" max="38" width="3" hidden="1" customWidth="1"/>
     <col min="39" max="42" width="3" customWidth="1"/>
     <col min="43" max="43" width="3" hidden="1" customWidth="1"/>
@@ -1987,13 +1976,13 @@
     <col min="49" max="52" width="3" customWidth="1"/>
     <col min="53" max="53" width="3" hidden="1" customWidth="1"/>
     <col min="54" max="58" width="3" customWidth="1"/>
-    <col min="59" max="59" width="5.75" customWidth="1"/>
+    <col min="59" max="59" width="5.765625" customWidth="1"/>
     <col min="60" max="63" width="3" customWidth="1"/>
-    <col min="64" max="64" width="5.375" customWidth="1"/>
+    <col min="64" max="64" width="5.3828125" customWidth="1"/>
     <col min="65" max="65" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2060,38 +2049,38 @@
       <c r="BL1" s="1"/>
       <c r="BM1" s="1"/>
     </row>
-    <row r="2" spans="1:65" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:65" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175"/>
-      <c r="N2" s="175"/>
-      <c r="O2" s="177"/>
-      <c r="P2" s="175"/>
-      <c r="Q2" s="175"/>
-      <c r="R2" s="175"/>
-      <c r="S2" s="175"/>
-      <c r="T2" s="175"/>
-      <c r="U2" s="175"/>
-      <c r="V2" s="175"/>
-      <c r="W2" s="175"/>
-      <c r="X2" s="175"/>
-      <c r="Y2" s="175"/>
-      <c r="Z2" s="175"/>
-      <c r="AA2" s="175"/>
-      <c r="AB2" s="175"/>
-      <c r="AC2" s="175"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="130"/>
+      <c r="P2" s="128"/>
+      <c r="Q2" s="128"/>
+      <c r="R2" s="128"/>
+      <c r="S2" s="128"/>
+      <c r="T2" s="128"/>
+      <c r="U2" s="128"/>
+      <c r="V2" s="128"/>
+      <c r="W2" s="128"/>
+      <c r="X2" s="128"/>
+      <c r="Y2" s="128"/>
+      <c r="Z2" s="128"/>
+      <c r="AA2" s="128"/>
+      <c r="AB2" s="128"/>
+      <c r="AC2" s="128"/>
       <c r="AD2" s="10"/>
       <c r="AE2" s="10"/>
       <c r="AF2" s="10"/>
@@ -2101,32 +2090,32 @@
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
-      <c r="AM2" s="126" t="s">
+      <c r="AM2" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="AN2" s="127"/>
-      <c r="AO2" s="127"/>
-      <c r="AP2" s="127"/>
-      <c r="AQ2" s="127"/>
-      <c r="AR2" s="127"/>
-      <c r="AS2" s="127"/>
-      <c r="AT2" s="170" t="s">
+      <c r="AN2" s="120"/>
+      <c r="AO2" s="120"/>
+      <c r="AP2" s="120"/>
+      <c r="AQ2" s="120"/>
+      <c r="AR2" s="120"/>
+      <c r="AS2" s="120"/>
+      <c r="AT2" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="AU2" s="127"/>
-      <c r="AV2" s="127"/>
-      <c r="AW2" s="127"/>
-      <c r="AX2" s="127"/>
-      <c r="AY2" s="127"/>
-      <c r="AZ2" s="127"/>
-      <c r="BA2" s="127"/>
-      <c r="BB2" s="127"/>
-      <c r="BC2" s="127"/>
+      <c r="AU2" s="120"/>
+      <c r="AV2" s="120"/>
+      <c r="AW2" s="120"/>
+      <c r="AX2" s="120"/>
+      <c r="AY2" s="120"/>
+      <c r="AZ2" s="120"/>
+      <c r="BA2" s="120"/>
+      <c r="BB2" s="120"/>
+      <c r="BC2" s="120"/>
       <c r="BK2" s="1"/>
       <c r="BL2" s="1"/>
       <c r="BM2" s="1"/>
     </row>
-    <row r="3" spans="1:65" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2193,7 +2182,7 @@
       <c r="BL3" s="1"/>
       <c r="BM3" s="1"/>
     </row>
-    <row r="4" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A4" s="1"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -2202,27 +2191,27 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="126" t="s">
+      <c r="I4" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="127"/>
-      <c r="N4" s="127"/>
-      <c r="O4" s="127"/>
-      <c r="P4" s="128">
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="120"/>
+      <c r="O4" s="120"/>
+      <c r="P4" s="131">
         <v>2023</v>
       </c>
-      <c r="Q4" s="127"/>
-      <c r="R4" s="127"/>
-      <c r="S4" s="127"/>
-      <c r="T4" s="127"/>
-      <c r="U4" s="127"/>
-      <c r="V4" s="127"/>
-      <c r="W4" s="127"/>
-      <c r="X4" s="127"/>
-      <c r="Y4" s="127"/>
+      <c r="Q4" s="120"/>
+      <c r="R4" s="120"/>
+      <c r="S4" s="120"/>
+      <c r="T4" s="120"/>
+      <c r="U4" s="120"/>
+      <c r="V4" s="120"/>
+      <c r="W4" s="120"/>
+      <c r="X4" s="120"/>
+      <c r="Y4" s="120"/>
       <c r="Z4" s="18"/>
       <c r="AA4" s="9"/>
       <c r="AB4" s="9"/>
@@ -2235,27 +2224,27 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
-      <c r="AM4" s="126" t="s">
+      <c r="AM4" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="AN4" s="127"/>
-      <c r="AO4" s="127"/>
-      <c r="AP4" s="127"/>
-      <c r="AQ4" s="127"/>
-      <c r="AR4" s="127"/>
-      <c r="AS4" s="127"/>
-      <c r="AT4" s="128">
+      <c r="AN4" s="120"/>
+      <c r="AO4" s="120"/>
+      <c r="AP4" s="120"/>
+      <c r="AQ4" s="120"/>
+      <c r="AR4" s="120"/>
+      <c r="AS4" s="120"/>
+      <c r="AT4" s="131">
         <v>2023</v>
       </c>
-      <c r="AU4" s="127"/>
-      <c r="AV4" s="127"/>
-      <c r="AW4" s="127"/>
-      <c r="AX4" s="127"/>
-      <c r="AY4" s="127"/>
-      <c r="AZ4" s="127"/>
-      <c r="BA4" s="127"/>
-      <c r="BB4" s="127"/>
-      <c r="BC4" s="127"/>
+      <c r="AU4" s="120"/>
+      <c r="AV4" s="120"/>
+      <c r="AW4" s="120"/>
+      <c r="AX4" s="120"/>
+      <c r="AY4" s="120"/>
+      <c r="AZ4" s="120"/>
+      <c r="BA4" s="120"/>
+      <c r="BB4" s="120"/>
+      <c r="BC4" s="120"/>
       <c r="BD4" s="1"/>
       <c r="BE4" s="1"/>
       <c r="BF4" s="1"/>
@@ -2267,7 +2256,7 @@
       <c r="BL4" s="1"/>
       <c r="BM4" s="1"/>
     </row>
-    <row r="5" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="19"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -2334,7 +2323,7 @@
       <c r="BL5" s="19"/>
       <c r="BM5" s="19"/>
     </row>
-    <row r="6" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22"/>
       <c r="B6" s="23" t="s">
         <v>1</v>
@@ -2347,73 +2336,73 @@
         <v>2</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="129" t="s">
+      <c r="I6" s="155" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="141"/>
-      <c r="K6" s="141"/>
-      <c r="L6" s="141"/>
-      <c r="M6" s="141"/>
-      <c r="N6" s="141"/>
-      <c r="O6" s="141"/>
-      <c r="P6" s="141"/>
-      <c r="Q6" s="141"/>
-      <c r="R6" s="141"/>
-      <c r="S6" s="141"/>
-      <c r="T6" s="141"/>
-      <c r="U6" s="151"/>
-      <c r="V6" s="129" t="s">
+      <c r="J6" s="133"/>
+      <c r="K6" s="133"/>
+      <c r="L6" s="133"/>
+      <c r="M6" s="133"/>
+      <c r="N6" s="133"/>
+      <c r="O6" s="133"/>
+      <c r="P6" s="133"/>
+      <c r="Q6" s="133"/>
+      <c r="R6" s="133"/>
+      <c r="S6" s="133"/>
+      <c r="T6" s="133"/>
+      <c r="U6" s="156"/>
+      <c r="V6" s="155" t="s">
         <v>4</v>
       </c>
-      <c r="W6" s="141"/>
-      <c r="X6" s="141"/>
-      <c r="Y6" s="141"/>
-      <c r="Z6" s="141"/>
-      <c r="AA6" s="141"/>
-      <c r="AB6" s="141"/>
-      <c r="AC6" s="141"/>
-      <c r="AD6" s="141"/>
-      <c r="AE6" s="141"/>
-      <c r="AF6" s="141"/>
-      <c r="AG6" s="141"/>
-      <c r="AH6" s="151"/>
-      <c r="AI6" s="129" t="s">
+      <c r="W6" s="133"/>
+      <c r="X6" s="133"/>
+      <c r="Y6" s="133"/>
+      <c r="Z6" s="133"/>
+      <c r="AA6" s="133"/>
+      <c r="AB6" s="133"/>
+      <c r="AC6" s="133"/>
+      <c r="AD6" s="133"/>
+      <c r="AE6" s="133"/>
+      <c r="AF6" s="133"/>
+      <c r="AG6" s="133"/>
+      <c r="AH6" s="156"/>
+      <c r="AI6" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="AJ6" s="130"/>
-      <c r="AK6" s="130"/>
-      <c r="AL6" s="130"/>
-      <c r="AM6" s="130"/>
-      <c r="AN6" s="130"/>
-      <c r="AO6" s="130"/>
-      <c r="AP6" s="130"/>
-      <c r="AQ6" s="130"/>
-      <c r="AR6" s="130"/>
-      <c r="AS6" s="130"/>
-      <c r="AT6" s="130"/>
-      <c r="AU6" s="130"/>
-      <c r="AV6" s="131"/>
-      <c r="AW6" s="129" t="s">
+      <c r="AJ6" s="171"/>
+      <c r="AK6" s="171"/>
+      <c r="AL6" s="171"/>
+      <c r="AM6" s="171"/>
+      <c r="AN6" s="171"/>
+      <c r="AO6" s="171"/>
+      <c r="AP6" s="171"/>
+      <c r="AQ6" s="171"/>
+      <c r="AR6" s="171"/>
+      <c r="AS6" s="171"/>
+      <c r="AT6" s="171"/>
+      <c r="AU6" s="171"/>
+      <c r="AV6" s="172"/>
+      <c r="AW6" s="155" t="s">
         <v>5</v>
       </c>
-      <c r="AX6" s="141"/>
-      <c r="AY6" s="141"/>
-      <c r="AZ6" s="141"/>
-      <c r="BA6" s="141"/>
-      <c r="BB6" s="141"/>
-      <c r="BC6" s="141"/>
-      <c r="BD6" s="141"/>
-      <c r="BE6" s="141"/>
-      <c r="BF6" s="141"/>
-      <c r="BG6" s="141"/>
-      <c r="BH6" s="141"/>
-      <c r="BI6" s="141"/>
-      <c r="BJ6" s="141"/>
-      <c r="BK6" s="151"/>
+      <c r="AX6" s="133"/>
+      <c r="AY6" s="133"/>
+      <c r="AZ6" s="133"/>
+      <c r="BA6" s="133"/>
+      <c r="BB6" s="133"/>
+      <c r="BC6" s="133"/>
+      <c r="BD6" s="133"/>
+      <c r="BE6" s="133"/>
+      <c r="BF6" s="133"/>
+      <c r="BG6" s="133"/>
+      <c r="BH6" s="133"/>
+      <c r="BI6" s="133"/>
+      <c r="BJ6" s="133"/>
+      <c r="BK6" s="156"/>
       <c r="BL6" s="19"/>
       <c r="BM6" s="19"/>
     </row>
-    <row r="7" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -2422,101 +2411,101 @@
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
-      <c r="I7" s="132" t="s">
+      <c r="I7" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="150"/>
-      <c r="K7" s="150"/>
-      <c r="L7" s="150"/>
-      <c r="M7" s="150"/>
-      <c r="N7" s="149" t="s">
+      <c r="J7" s="154"/>
+      <c r="K7" s="154"/>
+      <c r="L7" s="154"/>
+      <c r="M7" s="154"/>
+      <c r="N7" s="157" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="150"/>
-      <c r="P7" s="150"/>
-      <c r="Q7" s="150"/>
-      <c r="R7" s="133" t="s">
+      <c r="O7" s="154"/>
+      <c r="P7" s="154"/>
+      <c r="Q7" s="154"/>
+      <c r="R7" s="153" t="s">
         <v>8</v>
       </c>
-      <c r="S7" s="150"/>
-      <c r="T7" s="150"/>
-      <c r="U7" s="152"/>
-      <c r="V7" s="153" t="s">
+      <c r="S7" s="154"/>
+      <c r="T7" s="154"/>
+      <c r="U7" s="158"/>
+      <c r="V7" s="159" t="s">
         <v>9</v>
       </c>
-      <c r="W7" s="150"/>
-      <c r="X7" s="150"/>
-      <c r="Y7" s="150"/>
-      <c r="Z7" s="133" t="s">
+      <c r="W7" s="154"/>
+      <c r="X7" s="154"/>
+      <c r="Y7" s="154"/>
+      <c r="Z7" s="153" t="s">
         <v>10</v>
       </c>
-      <c r="AA7" s="150"/>
-      <c r="AB7" s="150"/>
-      <c r="AC7" s="150"/>
-      <c r="AD7" s="150"/>
-      <c r="AE7" s="149" t="s">
+      <c r="AA7" s="154"/>
+      <c r="AB7" s="154"/>
+      <c r="AC7" s="154"/>
+      <c r="AD7" s="154"/>
+      <c r="AE7" s="157" t="s">
         <v>11</v>
       </c>
-      <c r="AF7" s="150"/>
-      <c r="AG7" s="150"/>
-      <c r="AH7" s="152"/>
-      <c r="AI7" s="132" t="s">
+      <c r="AF7" s="154"/>
+      <c r="AG7" s="154"/>
+      <c r="AH7" s="158"/>
+      <c r="AI7" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="AJ7" s="133"/>
-      <c r="AK7" s="133"/>
-      <c r="AL7" s="133"/>
-      <c r="AM7" s="149" t="s">
+      <c r="AJ7" s="153"/>
+      <c r="AK7" s="153"/>
+      <c r="AL7" s="153"/>
+      <c r="AM7" s="157" t="s">
         <v>12</v>
       </c>
-      <c r="AN7" s="150"/>
-      <c r="AO7" s="150"/>
-      <c r="AP7" s="150"/>
-      <c r="AQ7" s="150"/>
-      <c r="AR7" s="133" t="s">
+      <c r="AN7" s="154"/>
+      <c r="AO7" s="154"/>
+      <c r="AP7" s="154"/>
+      <c r="AQ7" s="154"/>
+      <c r="AR7" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="AS7" s="150"/>
-      <c r="AT7" s="150"/>
-      <c r="AU7" s="150"/>
-      <c r="AV7" s="152"/>
-      <c r="AW7" s="153" t="s">
+      <c r="AS7" s="154"/>
+      <c r="AT7" s="154"/>
+      <c r="AU7" s="154"/>
+      <c r="AV7" s="158"/>
+      <c r="AW7" s="159" t="s">
         <v>14</v>
       </c>
-      <c r="AX7" s="150"/>
-      <c r="AY7" s="150"/>
-      <c r="AZ7" s="150"/>
-      <c r="BA7" s="150"/>
-      <c r="BB7" s="133" t="s">
+      <c r="AX7" s="154"/>
+      <c r="AY7" s="154"/>
+      <c r="AZ7" s="154"/>
+      <c r="BA7" s="154"/>
+      <c r="BB7" s="153" t="s">
         <v>15</v>
       </c>
-      <c r="BC7" s="150"/>
-      <c r="BD7" s="150"/>
-      <c r="BE7" s="150"/>
-      <c r="BF7" s="150"/>
-      <c r="BG7" s="149" t="s">
+      <c r="BC7" s="154"/>
+      <c r="BD7" s="154"/>
+      <c r="BE7" s="154"/>
+      <c r="BF7" s="154"/>
+      <c r="BG7" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="BH7" s="150"/>
-      <c r="BI7" s="150"/>
-      <c r="BJ7" s="150"/>
-      <c r="BK7" s="152"/>
+      <c r="BH7" s="154"/>
+      <c r="BI7" s="154"/>
+      <c r="BJ7" s="154"/>
+      <c r="BK7" s="158"/>
       <c r="BL7" s="25"/>
       <c r="BM7" s="25"/>
     </row>
-    <row r="8" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
-      <c r="D8" s="140" t="s">
+      <c r="D8" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="141"/>
+      <c r="E8" s="133"/>
       <c r="F8" s="30"/>
-      <c r="G8" s="140" t="s">
+      <c r="G8" s="161" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="141"/>
+      <c r="H8" s="133"/>
       <c r="I8" s="31" t="e">
         <f ca="1">DAY(FIRST_DAY_OF_YEAR($P4) + 7 * (COLUMN() - COLUMN($I8)))</f>
         <v>#NAME?</v>
@@ -2687,9 +2676,9 @@
       <c r="BL8" s="28"/>
       <c r="BM8" s="28"/>
     </row>
-    <row r="9" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="37"/>
-      <c r="B9" s="160">
+      <c r="B9" s="140">
         <v>1</v>
       </c>
       <c r="C9" s="38"/>
@@ -2698,10 +2687,10 @@
       </c>
       <c r="E9" s="143"/>
       <c r="F9" s="144"/>
-      <c r="G9" s="120" t="s">
+      <c r="G9" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="121"/>
+      <c r="H9" s="168"/>
       <c r="I9" s="39"/>
       <c r="J9" s="40"/>
       <c r="K9" s="58"/>
@@ -2728,7 +2717,7 @@
       <c r="AF9" s="43"/>
       <c r="AG9" s="43"/>
       <c r="AH9" s="43"/>
-      <c r="AI9" s="118"/>
+      <c r="AI9" s="165"/>
       <c r="AJ9" s="40"/>
       <c r="AK9" s="58"/>
       <c r="AL9" s="58"/>
@@ -2751,7 +2740,7 @@
       <c r="BD9" s="108"/>
       <c r="BE9" s="43"/>
       <c r="BF9" s="43"/>
-      <c r="BG9" s="118" t="s">
+      <c r="BG9" s="165" t="s">
         <v>17</v>
       </c>
       <c r="BH9" s="43"/>
@@ -2760,14 +2749,14 @@
       <c r="BK9" s="43"/>
       <c r="BM9" s="44"/>
     </row>
-    <row r="10" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19"/>
-      <c r="B10" s="141"/>
+      <c r="B10" s="133"/>
       <c r="C10" s="45"/>
-      <c r="D10" s="141"/>
-      <c r="E10" s="141"/>
-      <c r="F10" s="145"/>
-      <c r="G10" s="146" t="s">
+      <c r="D10" s="133"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="162" t="s">
         <v>26</v>
       </c>
       <c r="H10" s="123"/>
@@ -2797,14 +2786,14 @@
       <c r="AF10" s="48"/>
       <c r="AG10" s="48"/>
       <c r="AH10" s="48"/>
-      <c r="AI10" s="119"/>
+      <c r="AI10" s="166"/>
       <c r="AJ10" s="47"/>
       <c r="AK10" s="43"/>
       <c r="AL10" s="43"/>
       <c r="AM10" s="43"/>
       <c r="AN10" s="43"/>
       <c r="AO10" s="110"/>
-      <c r="AP10" s="183"/>
+      <c r="AP10" s="58"/>
       <c r="AQ10" s="58"/>
       <c r="AR10" s="58"/>
       <c r="AS10" s="58"/>
@@ -2821,24 +2810,24 @@
       <c r="BD10" s="109"/>
       <c r="BE10" s="48"/>
       <c r="BF10" s="48"/>
-      <c r="BG10" s="119"/>
+      <c r="BG10" s="166"/>
       <c r="BH10" s="48"/>
       <c r="BI10" s="48"/>
       <c r="BJ10" s="48"/>
       <c r="BK10" s="48"/>
       <c r="BM10" s="50"/>
     </row>
-    <row r="11" spans="1:65" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:65" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="19"/>
-      <c r="B11" s="141"/>
+      <c r="B11" s="133"/>
       <c r="C11" s="45"/>
-      <c r="D11" s="141"/>
-      <c r="E11" s="141"/>
-      <c r="F11" s="145"/>
-      <c r="G11" s="147" t="s">
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="148"/>
+      <c r="H11" s="164"/>
       <c r="I11" s="95"/>
       <c r="J11" s="51"/>
       <c r="K11" s="52"/>
@@ -2865,14 +2854,14 @@
       <c r="AF11" s="52"/>
       <c r="AG11" s="52"/>
       <c r="AH11" s="52"/>
-      <c r="AI11" s="119"/>
+      <c r="AI11" s="166"/>
       <c r="AJ11" s="51"/>
       <c r="AK11" s="52"/>
       <c r="AL11" s="52"/>
       <c r="AM11" s="52"/>
       <c r="AN11" s="52"/>
       <c r="AO11" s="111"/>
-      <c r="AP11" s="182"/>
+      <c r="AP11" s="52"/>
       <c r="AQ11" s="52"/>
       <c r="AR11" s="52"/>
       <c r="AS11" s="52"/>
@@ -2889,16 +2878,16 @@
       <c r="BD11" s="100"/>
       <c r="BE11" s="52"/>
       <c r="BF11" s="52"/>
-      <c r="BG11" s="119"/>
+      <c r="BG11" s="166"/>
       <c r="BH11" s="52"/>
       <c r="BI11" s="52"/>
       <c r="BJ11" s="52"/>
       <c r="BK11" s="52"/>
       <c r="BM11" s="50"/>
     </row>
-    <row r="12" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
-      <c r="B12" s="161">
+      <c r="B12" s="141">
         <v>2</v>
       </c>
       <c r="C12" s="45"/>
@@ -2907,7 +2896,7 @@
       </c>
       <c r="E12" s="143"/>
       <c r="F12" s="144"/>
-      <c r="G12" s="171" t="s">
+      <c r="G12" s="124" t="s">
         <v>27</v>
       </c>
       <c r="H12" s="123"/>
@@ -2937,21 +2926,21 @@
       <c r="AF12" s="55"/>
       <c r="AG12" s="55"/>
       <c r="AH12" s="55"/>
-      <c r="AI12" s="119"/>
+      <c r="AI12" s="166"/>
       <c r="AJ12" s="54"/>
       <c r="AK12" s="55"/>
       <c r="AL12" s="55"/>
       <c r="AM12" s="55"/>
       <c r="AN12" s="55"/>
       <c r="AO12" s="55"/>
-      <c r="AP12" s="185"/>
+      <c r="AP12" s="118"/>
       <c r="AQ12" s="55"/>
-      <c r="AR12" s="183"/>
+      <c r="AR12" s="58"/>
       <c r="AS12" s="55"/>
       <c r="AT12" s="101"/>
       <c r="AU12" s="58"/>
       <c r="AV12" s="49"/>
-      <c r="AW12" s="185"/>
+      <c r="AW12" s="118"/>
       <c r="AX12" s="58"/>
       <c r="AY12" s="58"/>
       <c r="AZ12" s="58"/>
@@ -2961,21 +2950,21 @@
       <c r="BD12" s="101"/>
       <c r="BE12" s="55"/>
       <c r="BF12" s="55"/>
-      <c r="BG12" s="119"/>
+      <c r="BG12" s="166"/>
       <c r="BH12" s="55"/>
       <c r="BI12" s="55"/>
       <c r="BJ12" s="55"/>
       <c r="BK12" s="55"/>
       <c r="BM12" s="19"/>
     </row>
-    <row r="13" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
-      <c r="B13" s="141"/>
+      <c r="B13" s="133"/>
       <c r="C13" s="45"/>
-      <c r="D13" s="141"/>
-      <c r="E13" s="141"/>
-      <c r="F13" s="145"/>
-      <c r="G13" s="171" t="s">
+      <c r="D13" s="133"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="134"/>
+      <c r="G13" s="124" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="123"/>
@@ -3005,21 +2994,21 @@
       <c r="AF13" s="58"/>
       <c r="AG13" s="58"/>
       <c r="AH13" s="58"/>
-      <c r="AI13" s="119"/>
+      <c r="AI13" s="166"/>
       <c r="AJ13" s="57"/>
       <c r="AK13" s="58"/>
       <c r="AL13" s="58"/>
       <c r="AM13" s="58"/>
       <c r="AN13" s="58"/>
       <c r="AO13" s="58"/>
-      <c r="AP13" s="185"/>
+      <c r="AP13" s="118"/>
       <c r="AQ13" s="58"/>
-      <c r="AR13" s="183"/>
+      <c r="AR13" s="58"/>
       <c r="AS13" s="58"/>
       <c r="AT13" s="99"/>
       <c r="AU13" s="58"/>
       <c r="AV13" s="59"/>
-      <c r="AW13" s="185"/>
+      <c r="AW13" s="118"/>
       <c r="AX13" s="58"/>
       <c r="AY13" s="58"/>
       <c r="AZ13" s="58"/>
@@ -3029,21 +3018,21 @@
       <c r="BD13" s="99"/>
       <c r="BE13" s="58"/>
       <c r="BF13" s="58"/>
-      <c r="BG13" s="119"/>
+      <c r="BG13" s="166"/>
       <c r="BH13" s="58"/>
       <c r="BI13" s="58"/>
       <c r="BJ13" s="58"/>
       <c r="BK13" s="58"/>
       <c r="BM13" s="19"/>
     </row>
-    <row r="14" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
-      <c r="B14" s="141"/>
+      <c r="B14" s="133"/>
       <c r="C14" s="45"/>
-      <c r="D14" s="141"/>
-      <c r="E14" s="141"/>
-      <c r="F14" s="145"/>
-      <c r="G14" s="171" t="s">
+      <c r="D14" s="133"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="134"/>
+      <c r="G14" s="124" t="s">
         <v>30</v>
       </c>
       <c r="H14" s="123"/>
@@ -3073,21 +3062,21 @@
       <c r="AF14" s="58"/>
       <c r="AG14" s="58"/>
       <c r="AH14" s="58"/>
-      <c r="AI14" s="119"/>
+      <c r="AI14" s="166"/>
       <c r="AJ14" s="57"/>
       <c r="AK14" s="58"/>
       <c r="AL14" s="58"/>
       <c r="AM14" s="58"/>
       <c r="AN14" s="58"/>
       <c r="AO14" s="58"/>
-      <c r="AP14" s="185"/>
+      <c r="AP14" s="118"/>
       <c r="AQ14" s="58"/>
       <c r="AR14" s="58"/>
-      <c r="AS14" s="183"/>
+      <c r="AS14" s="58"/>
       <c r="AT14" s="99"/>
       <c r="AU14" s="58"/>
       <c r="AV14" s="59"/>
-      <c r="AW14" s="185"/>
+      <c r="AW14" s="118"/>
       <c r="AX14" s="58"/>
       <c r="AY14" s="58"/>
       <c r="AZ14" s="58"/>
@@ -3097,21 +3086,21 @@
       <c r="BD14" s="99"/>
       <c r="BE14" s="58"/>
       <c r="BF14" s="58"/>
-      <c r="BG14" s="119"/>
+      <c r="BG14" s="166"/>
       <c r="BH14" s="58"/>
       <c r="BI14" s="58"/>
       <c r="BJ14" s="58"/>
       <c r="BK14" s="58"/>
       <c r="BM14" s="19"/>
     </row>
-    <row r="15" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
-      <c r="B15" s="141"/>
+      <c r="B15" s="133"/>
       <c r="C15" s="45"/>
-      <c r="D15" s="141"/>
-      <c r="E15" s="141"/>
-      <c r="F15" s="145"/>
-      <c r="G15" s="171" t="s">
+      <c r="D15" s="133"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="134"/>
+      <c r="G15" s="124" t="s">
         <v>31</v>
       </c>
       <c r="H15" s="123"/>
@@ -3141,21 +3130,21 @@
       <c r="AF15" s="58"/>
       <c r="AG15" s="58"/>
       <c r="AH15" s="58"/>
-      <c r="AI15" s="119"/>
+      <c r="AI15" s="166"/>
       <c r="AJ15" s="57"/>
       <c r="AK15" s="58"/>
       <c r="AL15" s="58"/>
       <c r="AM15" s="58"/>
       <c r="AN15" s="58"/>
       <c r="AO15" s="58"/>
-      <c r="AP15" s="185"/>
+      <c r="AP15" s="118"/>
       <c r="AQ15" s="58"/>
       <c r="AR15" s="58"/>
-      <c r="AS15" s="183"/>
+      <c r="AS15" s="58"/>
       <c r="AT15" s="99"/>
       <c r="AU15" s="58"/>
       <c r="AV15" s="59"/>
-      <c r="AW15" s="185"/>
+      <c r="AW15" s="118"/>
       <c r="AX15" s="58"/>
       <c r="AY15" s="58"/>
       <c r="AZ15" s="58"/>
@@ -3165,21 +3154,21 @@
       <c r="BD15" s="99"/>
       <c r="BE15" s="58"/>
       <c r="BF15" s="58"/>
-      <c r="BG15" s="119"/>
+      <c r="BG15" s="166"/>
       <c r="BH15" s="58"/>
       <c r="BI15" s="58"/>
       <c r="BJ15" s="58"/>
       <c r="BK15" s="58"/>
       <c r="BM15" s="19"/>
     </row>
-    <row r="16" spans="1:65" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
-      <c r="B16" s="141"/>
+      <c r="B16" s="133"/>
       <c r="C16" s="45"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="141"/>
-      <c r="F16" s="145"/>
-      <c r="G16" s="171"/>
+      <c r="D16" s="133"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="134"/>
+      <c r="G16" s="124"/>
       <c r="H16" s="123"/>
       <c r="I16" s="60"/>
       <c r="J16" s="61"/>
@@ -3207,7 +3196,7 @@
       <c r="AF16" s="62"/>
       <c r="AG16" s="62"/>
       <c r="AH16" s="62"/>
-      <c r="AI16" s="119"/>
+      <c r="AI16" s="166"/>
       <c r="AJ16" s="61"/>
       <c r="AK16" s="62"/>
       <c r="AL16" s="62"/>
@@ -3231,22 +3220,22 @@
       <c r="BD16" s="102"/>
       <c r="BE16" s="62"/>
       <c r="BF16" s="62"/>
-      <c r="BG16" s="119"/>
+      <c r="BG16" s="166"/>
       <c r="BH16" s="62"/>
       <c r="BI16" s="62"/>
       <c r="BJ16" s="62"/>
       <c r="BK16" s="62"/>
       <c r="BM16" s="19"/>
     </row>
-    <row r="17" spans="1:65" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:65" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="19"/>
-      <c r="B17" s="141"/>
+      <c r="B17" s="133"/>
       <c r="C17" s="64"/>
-      <c r="D17" s="162"/>
-      <c r="E17" s="162"/>
-      <c r="F17" s="163"/>
-      <c r="G17" s="172"/>
-      <c r="H17" s="173"/>
+      <c r="D17" s="145"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="146"/>
+      <c r="G17" s="125"/>
+      <c r="H17" s="126"/>
       <c r="I17" s="65"/>
       <c r="J17" s="66"/>
       <c r="K17" s="67"/>
@@ -3273,7 +3262,7 @@
       <c r="AF17" s="67"/>
       <c r="AG17" s="67"/>
       <c r="AH17" s="67"/>
-      <c r="AI17" s="119"/>
+      <c r="AI17" s="166"/>
       <c r="AJ17" s="66"/>
       <c r="AK17" s="67"/>
       <c r="AL17" s="67"/>
@@ -3297,24 +3286,24 @@
       <c r="BD17" s="103"/>
       <c r="BE17" s="67"/>
       <c r="BF17" s="67"/>
-      <c r="BG17" s="119"/>
+      <c r="BG17" s="166"/>
       <c r="BH17" s="67"/>
       <c r="BI17" s="67"/>
       <c r="BJ17" s="67"/>
       <c r="BK17" s="67"/>
       <c r="BM17" s="19"/>
     </row>
-    <row r="18" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
-      <c r="B18" s="164">
+      <c r="B18" s="147">
         <v>3</v>
       </c>
       <c r="C18" s="45"/>
-      <c r="D18" s="165" t="s">
+      <c r="D18" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="141"/>
-      <c r="F18" s="145"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="134"/>
       <c r="G18" s="122" t="s">
         <v>32</v>
       </c>
@@ -3345,7 +3334,7 @@
       <c r="AF18" s="71"/>
       <c r="AG18" s="71"/>
       <c r="AH18" s="71"/>
-      <c r="AI18" s="119"/>
+      <c r="AI18" s="166"/>
       <c r="AJ18" s="70"/>
       <c r="AK18" s="71"/>
       <c r="AL18" s="71"/>
@@ -3369,20 +3358,20 @@
       <c r="BD18" s="104"/>
       <c r="BE18" s="71"/>
       <c r="BF18" s="71"/>
-      <c r="BG18" s="119"/>
+      <c r="BG18" s="166"/>
       <c r="BH18" s="71"/>
       <c r="BI18" s="71"/>
       <c r="BJ18" s="71"/>
       <c r="BK18" s="71"/>
       <c r="BM18" s="19"/>
     </row>
-    <row r="19" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
-      <c r="B19" s="141"/>
+      <c r="B19" s="133"/>
       <c r="C19" s="45"/>
-      <c r="D19" s="141"/>
-      <c r="E19" s="141"/>
-      <c r="F19" s="145"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="134"/>
       <c r="G19" s="122" t="s">
         <v>33</v>
       </c>
@@ -3413,7 +3402,7 @@
       <c r="AF19" s="75"/>
       <c r="AG19" s="75"/>
       <c r="AH19" s="75"/>
-      <c r="AI19" s="119"/>
+      <c r="AI19" s="166"/>
       <c r="AJ19" s="74"/>
       <c r="AK19" s="75"/>
       <c r="AL19" s="75"/>
@@ -3427,7 +3416,7 @@
       <c r="AT19" s="105"/>
       <c r="AU19" s="75"/>
       <c r="AV19" s="76"/>
-      <c r="AW19" s="178"/>
+      <c r="AW19" s="71"/>
       <c r="AX19" s="75"/>
       <c r="AY19" s="75"/>
       <c r="AZ19" s="75"/>
@@ -3437,20 +3426,20 @@
       <c r="BD19" s="105"/>
       <c r="BE19" s="75"/>
       <c r="BF19" s="75"/>
-      <c r="BG19" s="119"/>
+      <c r="BG19" s="166"/>
       <c r="BH19" s="75"/>
       <c r="BI19" s="75"/>
       <c r="BJ19" s="75"/>
       <c r="BK19" s="75"/>
       <c r="BM19" s="19"/>
     </row>
-    <row r="20" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19"/>
-      <c r="B20" s="141"/>
+      <c r="B20" s="133"/>
       <c r="C20" s="45"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="145"/>
+      <c r="D20" s="133"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="134"/>
       <c r="G20" s="122" t="s">
         <v>36</v>
       </c>
@@ -3481,7 +3470,7 @@
       <c r="AF20" s="75"/>
       <c r="AG20" s="75"/>
       <c r="AH20" s="75"/>
-      <c r="AI20" s="119"/>
+      <c r="AI20" s="166"/>
       <c r="AJ20" s="74"/>
       <c r="AK20" s="75"/>
       <c r="AL20" s="75"/>
@@ -3495,8 +3484,8 @@
       <c r="AT20" s="105"/>
       <c r="AU20" s="75"/>
       <c r="AV20" s="76"/>
-      <c r="AW20" s="179"/>
-      <c r="AX20" s="180"/>
+      <c r="AW20" s="71"/>
+      <c r="AX20" s="71"/>
       <c r="AY20" s="75"/>
       <c r="AZ20" s="75"/>
       <c r="BA20" s="75"/>
@@ -3505,20 +3494,20 @@
       <c r="BD20" s="105"/>
       <c r="BE20" s="75"/>
       <c r="BF20" s="75"/>
-      <c r="BG20" s="119"/>
+      <c r="BG20" s="166"/>
       <c r="BH20" s="75"/>
       <c r="BI20" s="75"/>
       <c r="BJ20" s="75"/>
       <c r="BK20" s="75"/>
       <c r="BM20" s="19"/>
     </row>
-    <row r="21" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
-      <c r="B21" s="141"/>
+      <c r="B21" s="133"/>
       <c r="C21" s="45"/>
-      <c r="D21" s="141"/>
-      <c r="E21" s="141"/>
-      <c r="F21" s="145"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="134"/>
       <c r="G21" s="122" t="s">
         <v>37</v>
       </c>
@@ -3549,7 +3538,7 @@
       <c r="AF21" s="75"/>
       <c r="AG21" s="75"/>
       <c r="AH21" s="75"/>
-      <c r="AI21" s="119"/>
+      <c r="AI21" s="166"/>
       <c r="AJ21" s="74"/>
       <c r="AK21" s="75"/>
       <c r="AL21" s="75"/>
@@ -3563,7 +3552,7 @@
       <c r="AT21" s="105"/>
       <c r="AU21" s="75"/>
       <c r="AV21" s="76"/>
-      <c r="AW21" s="181"/>
+      <c r="AW21" s="71"/>
       <c r="AX21" s="75"/>
       <c r="AY21" s="75"/>
       <c r="AZ21" s="75"/>
@@ -3573,24 +3562,24 @@
       <c r="BD21" s="105"/>
       <c r="BE21" s="75"/>
       <c r="BF21" s="75"/>
-      <c r="BG21" s="119"/>
+      <c r="BG21" s="166"/>
       <c r="BH21" s="75"/>
       <c r="BI21" s="75"/>
       <c r="BJ21" s="75"/>
       <c r="BK21" s="75"/>
       <c r="BM21" s="19"/>
     </row>
-    <row r="22" spans="1:65" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:65" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="19"/>
-      <c r="B22" s="141"/>
+      <c r="B22" s="133"/>
       <c r="C22" s="77"/>
-      <c r="D22" s="166"/>
-      <c r="E22" s="166"/>
-      <c r="F22" s="167"/>
-      <c r="G22" s="134" t="s">
+      <c r="D22" s="149"/>
+      <c r="E22" s="149"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="135"/>
+      <c r="H22" s="174"/>
       <c r="I22" s="78"/>
       <c r="J22" s="79"/>
       <c r="K22" s="80"/>
@@ -3617,7 +3606,7 @@
       <c r="AF22" s="80"/>
       <c r="AG22" s="80"/>
       <c r="AH22" s="80"/>
-      <c r="AI22" s="119"/>
+      <c r="AI22" s="166"/>
       <c r="AJ22" s="79"/>
       <c r="AK22" s="80"/>
       <c r="AL22" s="80"/>
@@ -3629,7 +3618,7 @@
       <c r="AR22" s="112"/>
       <c r="AS22" s="80"/>
       <c r="AT22" s="106"/>
-      <c r="AU22" s="184"/>
+      <c r="AU22" s="80"/>
       <c r="AV22" s="81"/>
       <c r="AW22" s="80"/>
       <c r="AX22" s="80"/>
@@ -3641,25 +3630,25 @@
       <c r="BD22" s="106"/>
       <c r="BE22" s="80"/>
       <c r="BF22" s="80"/>
-      <c r="BG22" s="119"/>
+      <c r="BG22" s="166"/>
       <c r="BH22" s="80"/>
       <c r="BI22" s="80"/>
       <c r="BJ22" s="80"/>
       <c r="BK22" s="80"/>
       <c r="BM22" s="19"/>
     </row>
-    <row r="23" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="19"/>
-      <c r="B23" s="168">
+      <c r="B23" s="151">
         <v>4</v>
       </c>
       <c r="C23" s="45"/>
-      <c r="D23" s="154" t="s">
+      <c r="D23" s="132" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="141"/>
-      <c r="F23" s="145"/>
-      <c r="G23" s="136" t="s">
+      <c r="E23" s="133"/>
+      <c r="F23" s="134"/>
+      <c r="G23" s="175" t="s">
         <v>39</v>
       </c>
       <c r="H23" s="123"/>
@@ -3689,7 +3678,7 @@
       <c r="AF23" s="71"/>
       <c r="AG23" s="71"/>
       <c r="AH23" s="71"/>
-      <c r="AI23" s="119"/>
+      <c r="AI23" s="166"/>
       <c r="AJ23" s="70"/>
       <c r="AK23" s="71"/>
       <c r="AL23" s="71"/>
@@ -3713,21 +3702,21 @@
       <c r="BD23" s="104"/>
       <c r="BE23" s="71"/>
       <c r="BF23" s="71"/>
-      <c r="BG23" s="119"/>
+      <c r="BG23" s="166"/>
       <c r="BH23" s="71"/>
       <c r="BI23" s="71"/>
       <c r="BJ23" s="71"/>
       <c r="BK23" s="71"/>
       <c r="BM23" s="19"/>
     </row>
-    <row r="24" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="19"/>
-      <c r="B24" s="141"/>
+      <c r="B24" s="133"/>
       <c r="C24" s="45"/>
-      <c r="D24" s="141"/>
-      <c r="E24" s="141"/>
-      <c r="F24" s="145"/>
-      <c r="G24" s="136" t="s">
+      <c r="D24" s="133"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="134"/>
+      <c r="G24" s="175" t="s">
         <v>42</v>
       </c>
       <c r="H24" s="123"/>
@@ -3757,7 +3746,7 @@
       <c r="AF24" s="75"/>
       <c r="AG24" s="75"/>
       <c r="AH24" s="75"/>
-      <c r="AI24" s="119"/>
+      <c r="AI24" s="166"/>
       <c r="AJ24" s="74"/>
       <c r="AK24" s="75"/>
       <c r="AL24" s="75"/>
@@ -3781,21 +3770,21 @@
       <c r="BD24" s="105"/>
       <c r="BE24" s="75"/>
       <c r="BF24" s="75"/>
-      <c r="BG24" s="119"/>
+      <c r="BG24" s="166"/>
       <c r="BH24" s="75"/>
       <c r="BI24" s="75"/>
       <c r="BJ24" s="75"/>
       <c r="BK24" s="75"/>
       <c r="BM24" s="19"/>
     </row>
-    <row r="25" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="19"/>
-      <c r="B25" s="141"/>
+      <c r="B25" s="133"/>
       <c r="C25" s="45"/>
-      <c r="D25" s="141"/>
-      <c r="E25" s="141"/>
-      <c r="F25" s="145"/>
-      <c r="G25" s="136" t="s">
+      <c r="D25" s="133"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="175" t="s">
         <v>40</v>
       </c>
       <c r="H25" s="123"/>
@@ -3825,7 +3814,7 @@
       <c r="AF25" s="75"/>
       <c r="AG25" s="75"/>
       <c r="AH25" s="75"/>
-      <c r="AI25" s="119"/>
+      <c r="AI25" s="166"/>
       <c r="AJ25" s="74"/>
       <c r="AK25" s="75"/>
       <c r="AL25" s="75"/>
@@ -3849,24 +3838,24 @@
       <c r="BD25" s="105"/>
       <c r="BE25" s="75"/>
       <c r="BF25" s="75"/>
-      <c r="BG25" s="119"/>
+      <c r="BG25" s="166"/>
       <c r="BH25" s="75"/>
       <c r="BI25" s="75"/>
       <c r="BJ25" s="75"/>
       <c r="BK25" s="75"/>
       <c r="BM25" s="19"/>
     </row>
-    <row r="26" spans="1:65" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:65" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="19"/>
-      <c r="B26" s="141"/>
+      <c r="B26" s="133"/>
       <c r="C26" s="82"/>
-      <c r="D26" s="155"/>
-      <c r="E26" s="155"/>
-      <c r="F26" s="156"/>
-      <c r="G26" s="137" t="s">
+      <c r="D26" s="135"/>
+      <c r="E26" s="135"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="138"/>
+      <c r="H26" s="177"/>
       <c r="I26" s="83"/>
       <c r="J26" s="84"/>
       <c r="K26" s="85"/>
@@ -3893,7 +3882,7 @@
       <c r="AF26" s="85"/>
       <c r="AG26" s="85"/>
       <c r="AH26" s="85"/>
-      <c r="AI26" s="119"/>
+      <c r="AI26" s="166"/>
       <c r="AJ26" s="84"/>
       <c r="AK26" s="85"/>
       <c r="AL26" s="85"/>
@@ -3917,25 +3906,25 @@
       <c r="BD26" s="107"/>
       <c r="BE26" s="85"/>
       <c r="BF26" s="85"/>
-      <c r="BG26" s="119"/>
+      <c r="BG26" s="166"/>
       <c r="BH26" s="85"/>
       <c r="BI26" s="85"/>
       <c r="BJ26" s="85"/>
       <c r="BK26" s="85"/>
       <c r="BM26" s="19"/>
     </row>
-    <row r="27" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="19"/>
-      <c r="B27" s="169">
+      <c r="B27" s="152">
         <v>5</v>
       </c>
       <c r="C27" s="45"/>
-      <c r="D27" s="157" t="s">
+      <c r="D27" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="141"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="139" t="s">
+      <c r="E27" s="133"/>
+      <c r="F27" s="134"/>
+      <c r="G27" s="178" t="s">
         <v>43</v>
       </c>
       <c r="H27" s="123"/>
@@ -3965,7 +3954,7 @@
       <c r="AF27" s="71"/>
       <c r="AG27" s="71"/>
       <c r="AH27" s="71"/>
-      <c r="AI27" s="119"/>
+      <c r="AI27" s="166"/>
       <c r="AJ27" s="70"/>
       <c r="AK27" s="71"/>
       <c r="AL27" s="71"/>
@@ -3975,7 +3964,7 @@
       <c r="AP27" s="71"/>
       <c r="AQ27" s="71"/>
       <c r="AR27" s="71"/>
-      <c r="AS27" s="186"/>
+      <c r="AS27" s="116"/>
       <c r="AT27" s="104"/>
       <c r="AU27" s="71"/>
       <c r="AV27" s="72"/>
@@ -3989,21 +3978,21 @@
       <c r="BD27" s="104"/>
       <c r="BE27" s="71"/>
       <c r="BF27" s="71"/>
-      <c r="BG27" s="119"/>
+      <c r="BG27" s="166"/>
       <c r="BH27" s="71"/>
       <c r="BI27" s="71"/>
       <c r="BJ27" s="71"/>
       <c r="BK27" s="71"/>
       <c r="BM27" s="19"/>
     </row>
-    <row r="28" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="19"/>
-      <c r="B28" s="141"/>
+      <c r="B28" s="133"/>
       <c r="C28" s="45"/>
-      <c r="D28" s="141"/>
-      <c r="E28" s="141"/>
-      <c r="F28" s="145"/>
-      <c r="G28" s="139" t="s">
+      <c r="D28" s="133"/>
+      <c r="E28" s="133"/>
+      <c r="F28" s="134"/>
+      <c r="G28" s="178" t="s">
         <v>44</v>
       </c>
       <c r="H28" s="123"/>
@@ -4033,7 +4022,7 @@
       <c r="AF28" s="75"/>
       <c r="AG28" s="75"/>
       <c r="AH28" s="75"/>
-      <c r="AI28" s="119"/>
+      <c r="AI28" s="166"/>
       <c r="AJ28" s="74"/>
       <c r="AK28" s="75"/>
       <c r="AL28" s="75"/>
@@ -4043,7 +4032,7 @@
       <c r="AP28" s="75"/>
       <c r="AQ28" s="75"/>
       <c r="AR28" s="75"/>
-      <c r="AS28" s="186"/>
+      <c r="AS28" s="116"/>
       <c r="AT28" s="105"/>
       <c r="AU28" s="75"/>
       <c r="AV28" s="76"/>
@@ -4057,22 +4046,22 @@
       <c r="BD28" s="105"/>
       <c r="BE28" s="75"/>
       <c r="BF28" s="75"/>
-      <c r="BG28" s="119"/>
+      <c r="BG28" s="166"/>
       <c r="BH28" s="75"/>
       <c r="BI28" s="75"/>
       <c r="BJ28" s="75"/>
       <c r="BK28" s="75"/>
       <c r="BM28" s="19"/>
     </row>
-    <row r="29" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19"/>
-      <c r="B29" s="141"/>
+      <c r="B29" s="133"/>
       <c r="C29" s="87"/>
-      <c r="D29" s="158"/>
-      <c r="E29" s="158"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="124"/>
-      <c r="H29" s="125"/>
+      <c r="D29" s="138"/>
+      <c r="E29" s="138"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="169"/>
+      <c r="H29" s="170"/>
       <c r="I29" s="73"/>
       <c r="J29" s="74"/>
       <c r="K29" s="75"/>
@@ -4099,7 +4088,7 @@
       <c r="AF29" s="75"/>
       <c r="AG29" s="75"/>
       <c r="AH29" s="75"/>
-      <c r="AI29" s="119"/>
+      <c r="AI29" s="166"/>
       <c r="AJ29" s="74"/>
       <c r="AK29" s="75"/>
       <c r="AL29" s="75"/>
@@ -4123,14 +4112,14 @@
       <c r="BD29" s="105"/>
       <c r="BE29" s="75"/>
       <c r="BF29" s="75"/>
-      <c r="BG29" s="119"/>
+      <c r="BG29" s="166"/>
       <c r="BH29" s="75"/>
       <c r="BI29" s="75"/>
       <c r="BJ29" s="75"/>
       <c r="BK29" s="75"/>
       <c r="BM29" s="19"/>
     </row>
-    <row r="30" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="19"/>
       <c r="B30" s="88"/>
       <c r="C30" s="88"/>
@@ -4197,7 +4186,7 @@
       <c r="BL30" s="19"/>
       <c r="BM30" s="19"/>
     </row>
-    <row r="31" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="19"/>
       <c r="B31" s="88"/>
       <c r="C31" s="88"/>
@@ -4264,7 +4253,7 @@
       <c r="BL31" s="19"/>
       <c r="BM31" s="19"/>
     </row>
-    <row r="32" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="19"/>
       <c r="B32" s="88"/>
       <c r="C32" s="88"/>
@@ -4331,7 +4320,7 @@
       <c r="BL32" s="19"/>
       <c r="BM32" s="19"/>
     </row>
-    <row r="33" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="19"/>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -4398,7 +4387,7 @@
       <c r="BL33" s="19"/>
       <c r="BM33" s="19"/>
     </row>
-    <row r="34" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="19"/>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
@@ -4465,7 +4454,7 @@
       <c r="BL34" s="19"/>
       <c r="BM34" s="19"/>
     </row>
-    <row r="35" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:65" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="19"/>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
@@ -4534,6 +4523,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="BG9:BG29"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="AT4:BC4"/>
+    <mergeCell ref="AI6:AV6"/>
+    <mergeCell ref="AI7:AL7"/>
+    <mergeCell ref="AI9:AI29"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D9:F11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="I6:U6"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="Z7:AD7"/>
+    <mergeCell ref="V6:AH6"/>
+    <mergeCell ref="AW6:BK6"/>
+    <mergeCell ref="AM7:AQ7"/>
+    <mergeCell ref="AR7:AV7"/>
+    <mergeCell ref="AW7:BA7"/>
+    <mergeCell ref="BB7:BF7"/>
+    <mergeCell ref="BG7:BK7"/>
+    <mergeCell ref="AE7:AH7"/>
+    <mergeCell ref="D23:F26"/>
+    <mergeCell ref="D27:F29"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="D12:F17"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="D18:F22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B29"/>
     <mergeCell ref="AM2:AS2"/>
     <mergeCell ref="AT2:BC2"/>
     <mergeCell ref="G19:H19"/>
@@ -4550,50 +4583,6 @@
     <mergeCell ref="O2:AC2"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:Y4"/>
-    <mergeCell ref="D23:F26"/>
-    <mergeCell ref="D27:F29"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="D12:F17"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="D18:F22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="Z7:AD7"/>
-    <mergeCell ref="V6:AH6"/>
-    <mergeCell ref="AW6:BK6"/>
-    <mergeCell ref="AM7:AQ7"/>
-    <mergeCell ref="AR7:AV7"/>
-    <mergeCell ref="AW7:BA7"/>
-    <mergeCell ref="BB7:BF7"/>
-    <mergeCell ref="BG7:BK7"/>
-    <mergeCell ref="AE7:AH7"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="I6:U6"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D9:F11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="BG9:BG29"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="AT4:BC4"/>
-    <mergeCell ref="AI6:AV6"/>
-    <mergeCell ref="AI7:AL7"/>
-    <mergeCell ref="AI9:AI29"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>